<commit_message>
Static view level 1 -2
</commit_message>
<xml_diff>
--- a/DELIVERABLE/TASK_ASSIGN/BSS_TaskAssign.xlsx
+++ b/DELIVERABLE/TASK_ASSIGN/BSS_TaskAssign.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="264">
   <si>
     <t>ID</t>
   </si>
@@ -769,6 +769,60 @@
   </si>
   <si>
     <t>Writting rationel</t>
+  </si>
+  <si>
+    <t>Draw sequence diagram function "Manage Account"</t>
+  </si>
+  <si>
+    <t>Draw class diagram function "Manage Account"</t>
+  </si>
+  <si>
+    <t>Draw class diagram function "Manage News"</t>
+  </si>
+  <si>
+    <t>Draw class diagram function "Manage FAQ"</t>
+  </si>
+  <si>
+    <t>Draw class diagram function "Manage Homepage"</t>
+  </si>
+  <si>
+    <t>Draw class diagram function "Manage Categories"</t>
+  </si>
+  <si>
+    <t>Draw class diagram function "Manage Banners"</t>
+  </si>
+  <si>
+    <t>Draw class diagram function "Manage Popups"</t>
+  </si>
+  <si>
+    <t>Draw class diagram function "Manage Languages"</t>
+  </si>
+  <si>
+    <t>Draw class diagram function "Manage Examination"</t>
+  </si>
+  <si>
+    <t>Draw sequence diagram function "Manage News"</t>
+  </si>
+  <si>
+    <t>Draw sequence diagram function "Manage Categories"</t>
+  </si>
+  <si>
+    <t>Draw sequence diagram function "Manage Banners"</t>
+  </si>
+  <si>
+    <t>Draw sequence diagram function "Manage Popups"</t>
+  </si>
+  <si>
+    <t>Draw sequence diagram function "Manage Homepage"</t>
+  </si>
+  <si>
+    <t>Draw sequence diagram function "Manage Examination"</t>
+  </si>
+  <si>
+    <t>Draw sequence diagram function "Manage Language"</t>
+  </si>
+  <si>
+    <t>Draw sequence diagram function "Manage FAQ"</t>
   </si>
 </sst>
 </file>
@@ -1375,10 +1429,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:O241"/>
+  <dimension ref="B1:O265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C152" sqref="C152:C161"/>
+    <sheetView tabSelected="1" topLeftCell="A228" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D245" sqref="D245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8648,15 +8702,21 @@
       <c r="F227" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="G227" s="26"/>
-      <c r="H227" s="26"/>
+      <c r="G227" s="26">
+        <v>4</v>
+      </c>
+      <c r="H227" s="26">
+        <v>7</v>
+      </c>
       <c r="I227" s="26" t="s">
         <v>83</v>
       </c>
       <c r="J227" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="K227" s="27"/>
+      <c r="K227" s="27" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="228" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B228" s="19">
@@ -8674,15 +8734,21 @@
       <c r="F228" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="G228" s="20"/>
-      <c r="H228" s="20"/>
+      <c r="G228" s="20">
+        <v>2</v>
+      </c>
+      <c r="H228" s="20">
+        <v>4</v>
+      </c>
       <c r="I228" s="20" t="s">
         <v>83</v>
       </c>
       <c r="J228" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="K228" s="2"/>
+      <c r="K228" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="229" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B229" s="19">
@@ -8700,15 +8766,21 @@
       <c r="F229" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="G229" s="20"/>
-      <c r="H229" s="20"/>
+      <c r="G229" s="20">
+        <v>3</v>
+      </c>
+      <c r="H229" s="20">
+        <v>5</v>
+      </c>
       <c r="I229" s="20" t="s">
         <v>83</v>
       </c>
       <c r="J229" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K229" s="2"/>
+      <c r="K229" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="230" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B230" s="19">
@@ -8726,15 +8798,21 @@
       <c r="F230" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="G230" s="20"/>
-      <c r="H230" s="20"/>
+      <c r="G230" s="20">
+        <v>3</v>
+      </c>
+      <c r="H230" s="20">
+        <v>4</v>
+      </c>
       <c r="I230" s="20" t="s">
         <v>83</v>
       </c>
       <c r="J230" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="K230" s="2"/>
+      <c r="K230" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="231" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B231" s="19">
@@ -8752,7 +8830,9 @@
       <c r="F231" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="G231" s="20"/>
+      <c r="G231" s="20">
+        <v>3</v>
+      </c>
       <c r="H231" s="20"/>
       <c r="I231" s="20" t="s">
         <v>83</v>
@@ -8760,7 +8840,9 @@
       <c r="J231" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="K231" s="2"/>
+      <c r="K231" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="232" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B232" s="19">
@@ -8778,7 +8860,9 @@
       <c r="F232" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="G232" s="20"/>
+      <c r="G232" s="20">
+        <v>4</v>
+      </c>
       <c r="H232" s="20"/>
       <c r="I232" s="20" t="s">
         <v>83</v>
@@ -8806,15 +8890,21 @@
       <c r="F233" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="G233" s="20"/>
-      <c r="H233" s="20"/>
+      <c r="G233" s="20">
+        <v>3</v>
+      </c>
+      <c r="H233" s="20">
+        <v>3</v>
+      </c>
       <c r="I233" s="20" t="s">
         <v>83</v>
       </c>
       <c r="J233" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="K233" s="2"/>
+      <c r="K233" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="234" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B234" s="19">
@@ -8832,15 +8922,21 @@
       <c r="F234" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="G234" s="20"/>
-      <c r="H234" s="20"/>
+      <c r="G234" s="20">
+        <v>3</v>
+      </c>
+      <c r="H234" s="20">
+        <v>2</v>
+      </c>
       <c r="I234" s="20" t="s">
         <v>83</v>
       </c>
       <c r="J234" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="K234" s="2"/>
+      <c r="K234" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="235" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B235" s="19">
@@ -8858,15 +8954,21 @@
       <c r="F235" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="G235" s="20"/>
-      <c r="H235" s="20"/>
+      <c r="G235" s="20">
+        <v>4</v>
+      </c>
+      <c r="H235" s="20">
+        <v>5</v>
+      </c>
       <c r="I235" s="20" t="s">
         <v>83</v>
       </c>
       <c r="J235" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K235" s="2"/>
+      <c r="K235" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="236" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B236" s="19">
@@ -8884,82 +8986,682 @@
       <c r="F236" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="G236" s="20"/>
-      <c r="H236" s="20"/>
+      <c r="G236" s="20">
+        <v>4</v>
+      </c>
+      <c r="H236" s="20">
+        <v>3</v>
+      </c>
       <c r="I236" s="20" t="s">
         <v>83</v>
       </c>
       <c r="J236" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="K236" s="2"/>
-    </row>
-    <row r="237" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B237" s="19"/>
-      <c r="C237" s="20"/>
-      <c r="D237" s="2"/>
-      <c r="E237" s="2"/>
-      <c r="F237" s="20"/>
-      <c r="G237" s="20"/>
-      <c r="H237" s="20"/>
-      <c r="I237" s="20"/>
-      <c r="J237" s="20"/>
-      <c r="K237" s="2"/>
+      <c r="K236" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="237" spans="2:11" s="29" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B237" s="25">
+        <v>18</v>
+      </c>
+      <c r="C237" s="26">
+        <v>1</v>
+      </c>
+      <c r="D237" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E237" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F237" s="28">
+        <v>42888</v>
+      </c>
+      <c r="G237" s="26">
+        <v>3</v>
+      </c>
+      <c r="H237" s="26">
+        <v>4</v>
+      </c>
+      <c r="I237" s="28">
+        <v>42918</v>
+      </c>
+      <c r="J237" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="K237" s="27" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="238" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B238" s="19"/>
-      <c r="C238" s="20"/>
-      <c r="D238" s="2"/>
-      <c r="E238" s="2"/>
-      <c r="F238" s="20"/>
-      <c r="G238" s="20"/>
-      <c r="H238" s="20"/>
-      <c r="I238" s="20"/>
-      <c r="J238" s="20"/>
+      <c r="B238" s="19">
+        <v>18</v>
+      </c>
+      <c r="C238" s="20">
+        <v>2</v>
+      </c>
+      <c r="D238" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E238" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F238" s="24">
+        <v>42888</v>
+      </c>
+      <c r="G238" s="20">
+        <v>3</v>
+      </c>
+      <c r="H238" s="20">
+        <v>5</v>
+      </c>
+      <c r="I238" s="24">
+        <v>42949</v>
+      </c>
+      <c r="J238" s="20" t="s">
+        <v>39</v>
+      </c>
       <c r="K238" s="2"/>
     </row>
     <row r="239" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B239" s="19"/>
-      <c r="C239" s="20"/>
-      <c r="D239" s="2"/>
-      <c r="E239" s="2"/>
-      <c r="F239" s="20"/>
-      <c r="G239" s="20"/>
+      <c r="B239" s="19">
+        <v>18</v>
+      </c>
+      <c r="C239" s="20">
+        <v>3</v>
+      </c>
+      <c r="D239" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E239" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F239" s="24">
+        <v>42918</v>
+      </c>
+      <c r="G239" s="20">
+        <v>5</v>
+      </c>
       <c r="H239" s="20"/>
-      <c r="I239" s="20"/>
-      <c r="J239" s="20"/>
+      <c r="I239" s="24">
+        <v>42980</v>
+      </c>
+      <c r="J239" s="20" t="s">
+        <v>39</v>
+      </c>
       <c r="K239" s="2"/>
     </row>
     <row r="240" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B240" s="19"/>
-      <c r="C240" s="20"/>
-      <c r="D240" s="2"/>
-      <c r="E240" s="2"/>
-      <c r="F240" s="20"/>
+      <c r="B240" s="19">
+        <v>18</v>
+      </c>
+      <c r="C240" s="20">
+        <v>4</v>
+      </c>
+      <c r="D240" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E240" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F240" s="24">
+        <v>42918</v>
+      </c>
       <c r="G240" s="20"/>
       <c r="H240" s="20"/>
-      <c r="I240" s="20"/>
-      <c r="J240" s="20"/>
+      <c r="I240" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J240" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="K240" s="2"/>
     </row>
     <row r="241" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B241" s="19"/>
-      <c r="C241" s="20"/>
-      <c r="D241" s="2"/>
-      <c r="E241" s="2"/>
-      <c r="F241" s="20"/>
+      <c r="B241" s="19">
+        <v>18</v>
+      </c>
+      <c r="C241" s="20">
+        <v>5</v>
+      </c>
+      <c r="D241" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E241" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F241" s="24">
+        <v>42918</v>
+      </c>
       <c r="G241" s="20"/>
       <c r="H241" s="20"/>
-      <c r="I241" s="20"/>
-      <c r="J241" s="20"/>
+      <c r="I241" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J241" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="K241" s="2"/>
+    </row>
+    <row r="242" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B242" s="19">
+        <v>18</v>
+      </c>
+      <c r="C242" s="20">
+        <v>6</v>
+      </c>
+      <c r="D242" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E242" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F242" s="24">
+        <v>42918</v>
+      </c>
+      <c r="G242" s="20"/>
+      <c r="H242" s="20"/>
+      <c r="I242" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J242" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K242" s="2"/>
+    </row>
+    <row r="243" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B243" s="19">
+        <v>18</v>
+      </c>
+      <c r="C243" s="20">
+        <v>7</v>
+      </c>
+      <c r="D243" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E243" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F243" s="24">
+        <v>42918</v>
+      </c>
+      <c r="G243" s="20"/>
+      <c r="H243" s="20"/>
+      <c r="I243" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J243" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="K243" s="2"/>
+    </row>
+    <row r="244" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B244" s="19">
+        <v>18</v>
+      </c>
+      <c r="C244" s="20">
+        <v>8</v>
+      </c>
+      <c r="D244" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E244" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F244" s="24">
+        <v>42918</v>
+      </c>
+      <c r="G244" s="20"/>
+      <c r="H244" s="20"/>
+      <c r="I244" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J244" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="K244" s="2"/>
+    </row>
+    <row r="245" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B245" s="19">
+        <v>18</v>
+      </c>
+      <c r="C245" s="20">
+        <v>9</v>
+      </c>
+      <c r="D245" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E245" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F245" s="24">
+        <v>42918</v>
+      </c>
+      <c r="G245" s="20"/>
+      <c r="H245" s="20"/>
+      <c r="I245" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J245" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="K245" s="2"/>
+    </row>
+    <row r="246" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B246" s="19">
+        <v>18</v>
+      </c>
+      <c r="C246" s="20">
+        <v>10</v>
+      </c>
+      <c r="D246" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E246" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F246" s="24">
+        <v>42918</v>
+      </c>
+      <c r="G246" s="20"/>
+      <c r="H246" s="20"/>
+      <c r="I246" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J246" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K246" s="2"/>
+    </row>
+    <row r="247" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B247" s="19">
+        <v>18</v>
+      </c>
+      <c r="C247" s="20">
+        <v>11</v>
+      </c>
+      <c r="D247" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E247" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F247" s="24">
+        <v>42918</v>
+      </c>
+      <c r="G247" s="20"/>
+      <c r="H247" s="20"/>
+      <c r="I247" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J247" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="K247" s="2"/>
+    </row>
+    <row r="248" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B248" s="19">
+        <v>18</v>
+      </c>
+      <c r="C248" s="20">
+        <v>12</v>
+      </c>
+      <c r="D248" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E248" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F248" s="24">
+        <v>42918</v>
+      </c>
+      <c r="G248" s="20"/>
+      <c r="H248" s="20"/>
+      <c r="I248" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J248" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K248" s="2"/>
+    </row>
+    <row r="249" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B249" s="19">
+        <v>18</v>
+      </c>
+      <c r="C249" s="20">
+        <v>13</v>
+      </c>
+      <c r="D249" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E249" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F249" s="24">
+        <v>42918</v>
+      </c>
+      <c r="G249" s="20"/>
+      <c r="H249" s="20"/>
+      <c r="I249" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J249" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="K249" s="2"/>
+    </row>
+    <row r="250" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B250" s="19">
+        <v>18</v>
+      </c>
+      <c r="C250" s="20">
+        <v>14</v>
+      </c>
+      <c r="D250" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E250" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F250" s="24">
+        <v>42918</v>
+      </c>
+      <c r="G250" s="20"/>
+      <c r="H250" s="20"/>
+      <c r="I250" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J250" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="K250" s="2"/>
+    </row>
+    <row r="251" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B251" s="19">
+        <v>18</v>
+      </c>
+      <c r="C251" s="20">
+        <v>15</v>
+      </c>
+      <c r="D251" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E251" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F251" s="24">
+        <v>42918</v>
+      </c>
+      <c r="G251" s="20"/>
+      <c r="H251" s="20"/>
+      <c r="I251" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J251" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K251" s="2"/>
+    </row>
+    <row r="252" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B252" s="19">
+        <v>18</v>
+      </c>
+      <c r="C252" s="20">
+        <v>16</v>
+      </c>
+      <c r="D252" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E252" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F252" s="24">
+        <v>42918</v>
+      </c>
+      <c r="G252" s="20"/>
+      <c r="H252" s="20"/>
+      <c r="I252" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J252" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="K252" s="2"/>
+    </row>
+    <row r="253" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B253" s="19">
+        <v>18</v>
+      </c>
+      <c r="C253" s="20">
+        <v>17</v>
+      </c>
+      <c r="D253" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E253" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F253" s="24">
+        <v>42918</v>
+      </c>
+      <c r="G253" s="20"/>
+      <c r="H253" s="20"/>
+      <c r="I253" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J253" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K253" s="2"/>
+    </row>
+    <row r="254" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B254" s="19">
+        <v>18</v>
+      </c>
+      <c r="C254" s="20">
+        <v>18</v>
+      </c>
+      <c r="D254" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E254" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F254" s="24">
+        <v>42918</v>
+      </c>
+      <c r="G254" s="20"/>
+      <c r="H254" s="20"/>
+      <c r="I254" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J254" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="K254" s="2"/>
+    </row>
+    <row r="255" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B255" s="19">
+        <v>18</v>
+      </c>
+      <c r="C255" s="20">
+        <v>19</v>
+      </c>
+      <c r="D255" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E255" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F255" s="24">
+        <v>42918</v>
+      </c>
+      <c r="G255" s="20"/>
+      <c r="H255" s="20"/>
+      <c r="I255" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J255" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="K255" s="2"/>
+    </row>
+    <row r="256" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B256" s="19">
+        <v>18</v>
+      </c>
+      <c r="C256" s="20">
+        <v>20</v>
+      </c>
+      <c r="D256" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E256" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F256" s="24">
+        <v>42918</v>
+      </c>
+      <c r="G256" s="20"/>
+      <c r="H256" s="20"/>
+      <c r="I256" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J256" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K256" s="2"/>
+    </row>
+    <row r="257" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B257" s="19">
+        <v>18</v>
+      </c>
+      <c r="C257" s="20">
+        <v>21</v>
+      </c>
+      <c r="D257" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E257" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F257" s="24">
+        <v>42918</v>
+      </c>
+      <c r="G257" s="20"/>
+      <c r="H257" s="20"/>
+      <c r="I257" s="24">
+        <v>43010</v>
+      </c>
+      <c r="J257" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K257" s="2"/>
+    </row>
+    <row r="258" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B258" s="19"/>
+      <c r="C258" s="20"/>
+      <c r="D258" s="2"/>
+      <c r="E258" s="2"/>
+      <c r="F258" s="20"/>
+      <c r="G258" s="20"/>
+      <c r="H258" s="20"/>
+      <c r="I258" s="20"/>
+      <c r="J258" s="20"/>
+      <c r="K258" s="2"/>
+    </row>
+    <row r="259" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B259" s="19"/>
+      <c r="C259" s="20"/>
+      <c r="D259" s="2"/>
+      <c r="E259" s="2"/>
+      <c r="F259" s="20"/>
+      <c r="G259" s="20"/>
+      <c r="H259" s="20"/>
+      <c r="I259" s="20"/>
+      <c r="J259" s="20"/>
+      <c r="K259" s="2"/>
+    </row>
+    <row r="260" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B260" s="19"/>
+      <c r="C260" s="20"/>
+      <c r="D260" s="2"/>
+      <c r="E260" s="2"/>
+      <c r="F260" s="20"/>
+      <c r="G260" s="20"/>
+      <c r="H260" s="20"/>
+      <c r="I260" s="20"/>
+      <c r="J260" s="20"/>
+      <c r="K260" s="2"/>
+    </row>
+    <row r="261" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B261" s="19"/>
+      <c r="C261" s="20"/>
+      <c r="D261" s="2"/>
+      <c r="E261" s="2"/>
+      <c r="F261" s="20"/>
+      <c r="G261" s="20"/>
+      <c r="H261" s="20"/>
+      <c r="I261" s="20"/>
+      <c r="J261" s="20"/>
+      <c r="K261" s="2"/>
+    </row>
+    <row r="262" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B262" s="19"/>
+      <c r="C262" s="20"/>
+      <c r="D262" s="2"/>
+      <c r="E262" s="2"/>
+      <c r="F262" s="20"/>
+      <c r="G262" s="20"/>
+      <c r="H262" s="20"/>
+      <c r="I262" s="20"/>
+      <c r="J262" s="20"/>
+      <c r="K262" s="2"/>
+    </row>
+    <row r="263" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B263" s="19"/>
+      <c r="C263" s="20"/>
+      <c r="D263" s="2"/>
+      <c r="E263" s="2"/>
+      <c r="F263" s="20"/>
+      <c r="G263" s="20"/>
+      <c r="H263" s="20"/>
+      <c r="I263" s="20"/>
+      <c r="J263" s="20"/>
+      <c r="K263" s="2"/>
+    </row>
+    <row r="264" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B264" s="19"/>
+      <c r="C264" s="20"/>
+      <c r="D264" s="2"/>
+      <c r="E264" s="2"/>
+      <c r="F264" s="20"/>
+      <c r="G264" s="20"/>
+      <c r="H264" s="20"/>
+      <c r="I264" s="20"/>
+      <c r="J264" s="20"/>
+      <c r="K264" s="2"/>
+    </row>
+    <row r="265" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B265" s="19"/>
+      <c r="C265" s="20"/>
+      <c r="D265" s="2"/>
+      <c r="E265" s="2"/>
+      <c r="F265" s="20"/>
+      <c r="G265" s="20"/>
+      <c r="H265" s="20"/>
+      <c r="I265" s="20"/>
+      <c r="J265" s="20"/>
+      <c r="K265" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N4">
       <formula1>Trangthai</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K241">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K265">
       <formula1>sta</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
estimate and actual time
</commit_message>
<xml_diff>
--- a/DELIVERABLE/TASK_ASSIGN/BSS_TaskAssign.xlsx
+++ b/DELIVERABLE/TASK_ASSIGN/BSS_TaskAssign.xlsx
@@ -1415,7 +1415,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1426,8 +1426,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:O265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A228" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G253" sqref="G253"/>
+    <sheetView tabSelected="1" topLeftCell="A234" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G256" sqref="G256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9443,8 +9443,12 @@
       <c r="F253" s="24">
         <v>42918</v>
       </c>
-      <c r="G253" s="20"/>
-      <c r="H253" s="20"/>
+      <c r="G253" s="20">
+        <v>7</v>
+      </c>
+      <c r="H253" s="20">
+        <v>8</v>
+      </c>
       <c r="I253" s="24">
         <v>43010</v>
       </c>

</xml_diff>